<commit_message>
fix: fill missing rate-card prices and seed inactive defaults
Context:
- Some models had active rate-card rows with raw_cost_per_unit_kopeks=0, leading to free usage and incorrect public pricing.
- New installs could also get active 0-priced defaults from the billing seed.

Changes:
- Update `.memory_bank/images/rate-cards-all_units_template (2)-filled.xlsx` to remove active zero prices (fill missing rates; disable irrelevant modalities).
- Seed default rate cards as inactive in `backend/open_webui/utils/billing_seed.py`.
- Add regression test `backend/open_webui/test/apps/webui/utils/test_billing_seed.py`.
- Log task update in `.memory_bank/branch_updates/2026-02-02-vk-1089-.md`.

Tests:
- pytest -q backend/open_webui/test/apps/webui/utils/test_billing_seed.py

Risks:
- New installs will require an admin import/apply to activate pricing (intended to avoid free pricing by default).
</commit_message>
<xml_diff>
--- a/.memory_bank/images/rate-cards-all_units_template (2)-filled.xlsx
+++ b/.memory_bank/images/rate-cards-all_units_template (2)-filled.xlsx
@@ -510,14 +510,11 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+        <v>7</v>
+      </c>
       <c r="I2" t="n">
         <v>1</v>
       </c>
-      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -544,14 +541,11 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+        <v>11</v>
+      </c>
       <c r="I3" t="n">
         <v>1</v>
       </c>
-      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -575,17 +569,11 @@
         </is>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I4" t="n">
         <v>1</v>
       </c>
-      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -609,17 +597,11 @@
         </is>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I5" t="n">
         <v>1</v>
       </c>
-      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -645,11 +627,6 @@
       <c r="E6" t="b">
         <v>0</v>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -676,14 +653,11 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+        <v>7</v>
+      </c>
       <c r="I7" t="n">
         <v>1</v>
       </c>
-      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -710,14 +684,11 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+        <v>11</v>
+      </c>
       <c r="I8" t="n">
         <v>1</v>
       </c>
-      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -741,17 +712,11 @@
         </is>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
-      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -775,17 +740,11 @@
         </is>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I10" t="n">
         <v>1</v>
       </c>
-      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -811,11 +770,6 @@
       <c r="E11" t="b">
         <v>0</v>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -844,8 +798,6 @@
       <c r="F12" t="n">
         <v>7</v>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
         <v>0</v>
       </c>
@@ -882,8 +834,6 @@
       <c r="F13" t="n">
         <v>63</v>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
         <v>0</v>
       </c>
@@ -917,11 +867,6 @@
       <c r="E14" t="b">
         <v>0</v>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -947,11 +892,6 @@
       <c r="E15" t="b">
         <v>0</v>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -977,11 +917,6 @@
       <c r="E16" t="b">
         <v>0</v>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1010,12 +945,9 @@
       <c r="F17" t="n">
         <v>100</v>
       </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
         <v>0</v>
       </c>
-      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1044,12 +976,9 @@
       <c r="F18" t="n">
         <v>100</v>
       </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
         <v>0</v>
       </c>
-      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1075,11 +1004,6 @@
       <c r="E19" t="b">
         <v>0</v>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1105,11 +1029,6 @@
       <c r="E20" t="b">
         <v>0</v>
       </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1135,11 +1054,6 @@
       <c r="E21" t="b">
         <v>0</v>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1166,14 +1080,11 @@
         <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+        <v>7</v>
+      </c>
       <c r="I22" t="n">
         <v>1</v>
       </c>
-      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1200,14 +1111,11 @@
         <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+        <v>63</v>
+      </c>
       <c r="I23" t="n">
         <v>1</v>
       </c>
-      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1231,17 +1139,11 @@
         </is>
       </c>
       <c r="E24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I24" t="n">
         <v>1</v>
       </c>
-      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1265,17 +1167,11 @@
         </is>
       </c>
       <c r="E25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I25" t="n">
         <v>1</v>
       </c>
-      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1301,11 +1197,6 @@
       <c r="E26" t="b">
         <v>0</v>
       </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1334,8 +1225,6 @@
       <c r="F27" t="n">
         <v>29</v>
       </c>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
       <c r="I27" t="n">
         <v>1</v>
       </c>
@@ -1372,8 +1261,6 @@
       <c r="F28" t="n">
         <v>250</v>
       </c>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
         <v>1</v>
       </c>
@@ -1405,17 +1292,11 @@
         </is>
       </c>
       <c r="E29" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I29" t="n">
         <v>1</v>
       </c>
-      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1439,17 +1320,11 @@
         </is>
       </c>
       <c r="E30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I30" t="n">
         <v>1</v>
       </c>
-      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1475,11 +1350,6 @@
       <c r="E31" t="b">
         <v>0</v>
       </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1508,8 +1378,6 @@
       <c r="F32" t="n">
         <v>12</v>
       </c>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
         <v>1</v>
       </c>
@@ -1546,8 +1414,6 @@
       <c r="F33" t="n">
         <v>75</v>
       </c>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
       <c r="I33" t="n">
         <v>1</v>
       </c>
@@ -1579,17 +1445,11 @@
         </is>
       </c>
       <c r="E34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I34" t="n">
         <v>1</v>
       </c>
-      <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1613,17 +1473,11 @@
         </is>
       </c>
       <c r="E35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I35" t="n">
         <v>1</v>
       </c>
-      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1649,11 +1503,6 @@
       <c r="E36" t="b">
         <v>0</v>
       </c>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1680,14 +1529,11 @@
         <v>1</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
+        <v>23</v>
+      </c>
       <c r="I37" t="n">
         <v>1</v>
       </c>
-      <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1714,14 +1560,11 @@
         <v>1</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
+        <v>150</v>
+      </c>
       <c r="I38" t="n">
         <v>1</v>
       </c>
-      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1745,17 +1588,11 @@
         </is>
       </c>
       <c r="E39" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I39" t="n">
         <v>1</v>
       </c>
-      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1779,17 +1616,11 @@
         </is>
       </c>
       <c r="E40" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I40" t="n">
         <v>1</v>
       </c>
-      <c r="J40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1815,11 +1646,6 @@
       <c r="E41" t="b">
         <v>0</v>
       </c>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1848,8 +1674,6 @@
       <c r="F42" t="n">
         <v>23</v>
       </c>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
       <c r="I42" t="n">
         <v>1</v>
       </c>
@@ -1886,8 +1710,6 @@
       <c r="F43" t="n">
         <v>150</v>
       </c>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
       <c r="I43" t="n">
         <v>1</v>
       </c>
@@ -1919,17 +1741,11 @@
         </is>
       </c>
       <c r="E44" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I44" t="n">
         <v>1</v>
       </c>
-      <c r="J44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1953,17 +1769,11 @@
         </is>
       </c>
       <c r="E45" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I45" t="n">
         <v>1</v>
       </c>
-      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1989,11 +1799,6 @@
       <c r="E46" t="b">
         <v>0</v>
       </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2017,17 +1822,11 @@
         </is>
       </c>
       <c r="E47" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" t="n">
-        <v>0</v>
-      </c>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I47" t="n">
         <v>1</v>
       </c>
-      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2051,17 +1850,11 @@
         </is>
       </c>
       <c r="E48" t="b">
-        <v>1</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I48" t="n">
         <v>1</v>
       </c>
-      <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2085,17 +1878,11 @@
         </is>
       </c>
       <c r="E49" t="b">
-        <v>1</v>
-      </c>
-      <c r="F49" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I49" t="n">
         <v>1</v>
       </c>
-      <c r="J49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2119,17 +1906,11 @@
         </is>
       </c>
       <c r="E50" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I50" t="n">
         <v>1</v>
       </c>
-      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2155,11 +1936,6 @@
       <c r="E51" t="b">
         <v>0</v>
       </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
-      <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2183,17 +1959,11 @@
         </is>
       </c>
       <c r="E52" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I52" t="n">
         <v>1</v>
       </c>
-      <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2217,17 +1987,11 @@
         </is>
       </c>
       <c r="E53" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" t="n">
-        <v>0</v>
-      </c>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I53" t="n">
         <v>1</v>
       </c>
-      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2251,17 +2015,11 @@
         </is>
       </c>
       <c r="E54" t="b">
-        <v>1</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I54" t="n">
         <v>1</v>
       </c>
-      <c r="J54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2285,17 +2043,11 @@
         </is>
       </c>
       <c r="E55" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I55" t="n">
         <v>1</v>
       </c>
-      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2321,11 +2073,6 @@
       <c r="E56" t="b">
         <v>0</v>
       </c>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
-      <c r="J56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2349,17 +2096,11 @@
         </is>
       </c>
       <c r="E57" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" t="n">
-        <v>0</v>
-      </c>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I57" t="n">
         <v>1</v>
       </c>
-      <c r="J57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2383,17 +2124,11 @@
         </is>
       </c>
       <c r="E58" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I58" t="n">
         <v>1</v>
       </c>
-      <c r="J58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2417,17 +2152,11 @@
         </is>
       </c>
       <c r="E59" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" t="inlineStr"/>
-      <c r="H59" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I59" t="n">
         <v>1</v>
       </c>
-      <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2451,17 +2180,11 @@
         </is>
       </c>
       <c r="E60" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" t="n">
-        <v>0</v>
-      </c>
-      <c r="G60" t="inlineStr"/>
-      <c r="H60" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I60" t="n">
         <v>1</v>
       </c>
-      <c r="J60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2487,11 +2210,6 @@
       <c r="E61" t="b">
         <v>0</v>
       </c>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
-      <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
-      <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2515,17 +2233,11 @@
         </is>
       </c>
       <c r="E62" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" t="n">
-        <v>0</v>
-      </c>
-      <c r="G62" t="inlineStr"/>
-      <c r="H62" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I62" t="n">
         <v>1</v>
       </c>
-      <c r="J62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2549,17 +2261,11 @@
         </is>
       </c>
       <c r="E63" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G63" t="inlineStr"/>
-      <c r="H63" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I63" t="n">
         <v>1</v>
       </c>
-      <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2583,17 +2289,11 @@
         </is>
       </c>
       <c r="E64" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" t="n">
-        <v>0</v>
-      </c>
-      <c r="G64" t="inlineStr"/>
-      <c r="H64" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I64" t="n">
         <v>1</v>
       </c>
-      <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2617,17 +2317,11 @@
         </is>
       </c>
       <c r="E65" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" t="n">
-        <v>0</v>
-      </c>
-      <c r="G65" t="inlineStr"/>
-      <c r="H65" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I65" t="n">
         <v>1</v>
       </c>
-      <c r="J65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2653,11 +2347,6 @@
       <c r="E66" t="b">
         <v>0</v>
       </c>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="inlineStr"/>
-      <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr"/>
-      <c r="J66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2681,17 +2370,11 @@
         </is>
       </c>
       <c r="E67" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" t="n">
-        <v>0</v>
-      </c>
-      <c r="G67" t="inlineStr"/>
-      <c r="H67" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I67" t="n">
         <v>1</v>
       </c>
-      <c r="J67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2715,17 +2398,11 @@
         </is>
       </c>
       <c r="E68" t="b">
-        <v>1</v>
-      </c>
-      <c r="F68" t="n">
-        <v>0</v>
-      </c>
-      <c r="G68" t="inlineStr"/>
-      <c r="H68" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I68" t="n">
         <v>1</v>
       </c>
-      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2749,17 +2426,11 @@
         </is>
       </c>
       <c r="E69" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" t="n">
-        <v>0</v>
-      </c>
-      <c r="G69" t="inlineStr"/>
-      <c r="H69" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I69" t="n">
         <v>1</v>
       </c>
-      <c r="J69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2783,17 +2454,11 @@
         </is>
       </c>
       <c r="E70" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" t="n">
-        <v>0</v>
-      </c>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I70" t="n">
         <v>1</v>
       </c>
-      <c r="J70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2819,11 +2484,6 @@
       <c r="E71" t="b">
         <v>0</v>
       </c>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr"/>
-      <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr"/>
-      <c r="J71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2852,8 +2512,6 @@
       <c r="F72" t="n">
         <v>46</v>
       </c>
-      <c r="G72" t="inlineStr"/>
-      <c r="H72" t="inlineStr"/>
       <c r="I72" t="n">
         <v>1</v>
       </c>
@@ -2890,8 +2548,6 @@
       <c r="F73" t="n">
         <v>200</v>
       </c>
-      <c r="G73" t="inlineStr"/>
-      <c r="H73" t="inlineStr"/>
       <c r="I73" t="n">
         <v>1</v>
       </c>
@@ -2923,17 +2579,11 @@
         </is>
       </c>
       <c r="E74" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" t="n">
-        <v>0</v>
-      </c>
-      <c r="G74" t="inlineStr"/>
-      <c r="H74" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I74" t="n">
         <v>1</v>
       </c>
-      <c r="J74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2957,17 +2607,11 @@
         </is>
       </c>
       <c r="E75" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" t="n">
-        <v>0</v>
-      </c>
-      <c r="G75" t="inlineStr"/>
-      <c r="H75" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I75" t="n">
         <v>1</v>
       </c>
-      <c r="J75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2993,11 +2637,6 @@
       <c r="E76" t="b">
         <v>0</v>
       </c>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr"/>
-      <c r="H76" t="inlineStr"/>
-      <c r="I76" t="inlineStr"/>
-      <c r="J76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3026,8 +2665,6 @@
       <c r="F77" t="n">
         <v>10</v>
       </c>
-      <c r="G77" t="inlineStr"/>
-      <c r="H77" t="inlineStr"/>
       <c r="I77" t="n">
         <v>1</v>
       </c>
@@ -3064,8 +2701,6 @@
       <c r="F78" t="n">
         <v>40</v>
       </c>
-      <c r="G78" t="inlineStr"/>
-      <c r="H78" t="inlineStr"/>
       <c r="I78" t="n">
         <v>1</v>
       </c>
@@ -3097,17 +2732,11 @@
         </is>
       </c>
       <c r="E79" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" t="n">
-        <v>0</v>
-      </c>
-      <c r="G79" t="inlineStr"/>
-      <c r="H79" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I79" t="n">
         <v>1</v>
       </c>
-      <c r="J79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3131,17 +2760,11 @@
         </is>
       </c>
       <c r="E80" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" t="n">
-        <v>0</v>
-      </c>
-      <c r="G80" t="inlineStr"/>
-      <c r="H80" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I80" t="n">
         <v>1</v>
       </c>
-      <c r="J80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3167,11 +2790,6 @@
       <c r="E81" t="b">
         <v>0</v>
       </c>
-      <c r="F81" t="inlineStr"/>
-      <c r="G81" t="inlineStr"/>
-      <c r="H81" t="inlineStr"/>
-      <c r="I81" t="inlineStr"/>
-      <c r="J81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3200,8 +2818,6 @@
       <c r="F82" t="n">
         <v>3</v>
       </c>
-      <c r="G82" t="inlineStr"/>
-      <c r="H82" t="inlineStr"/>
       <c r="I82" t="n">
         <v>1</v>
       </c>
@@ -3238,8 +2854,6 @@
       <c r="F83" t="n">
         <v>10</v>
       </c>
-      <c r="G83" t="inlineStr"/>
-      <c r="H83" t="inlineStr"/>
       <c r="I83" t="n">
         <v>1</v>
       </c>
@@ -3271,17 +2885,11 @@
         </is>
       </c>
       <c r="E84" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" t="n">
-        <v>0</v>
-      </c>
-      <c r="G84" t="inlineStr"/>
-      <c r="H84" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I84" t="n">
         <v>1</v>
       </c>
-      <c r="J84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3305,17 +2913,11 @@
         </is>
       </c>
       <c r="E85" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" t="n">
-        <v>0</v>
-      </c>
-      <c r="G85" t="inlineStr"/>
-      <c r="H85" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I85" t="n">
         <v>1</v>
       </c>
-      <c r="J85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3341,11 +2943,6 @@
       <c r="E86" t="b">
         <v>0</v>
       </c>
-      <c r="F86" t="inlineStr"/>
-      <c r="G86" t="inlineStr"/>
-      <c r="H86" t="inlineStr"/>
-      <c r="I86" t="inlineStr"/>
-      <c r="J86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3374,8 +2971,6 @@
       <c r="F87" t="n">
         <v>58</v>
       </c>
-      <c r="G87" t="inlineStr"/>
-      <c r="H87" t="inlineStr"/>
       <c r="I87" t="n">
         <v>1</v>
       </c>
@@ -3412,8 +3007,6 @@
       <c r="F88" t="n">
         <v>250</v>
       </c>
-      <c r="G88" t="inlineStr"/>
-      <c r="H88" t="inlineStr"/>
       <c r="I88" t="n">
         <v>1</v>
       </c>
@@ -3445,17 +3038,11 @@
         </is>
       </c>
       <c r="E89" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" t="n">
-        <v>0</v>
-      </c>
-      <c r="G89" t="inlineStr"/>
-      <c r="H89" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I89" t="n">
         <v>1</v>
       </c>
-      <c r="J89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3479,17 +3066,11 @@
         </is>
       </c>
       <c r="E90" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G90" t="inlineStr"/>
-      <c r="H90" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I90" t="n">
         <v>1</v>
       </c>
-      <c r="J90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3515,11 +3096,6 @@
       <c r="E91" t="b">
         <v>0</v>
       </c>
-      <c r="F91" t="inlineStr"/>
-      <c r="G91" t="inlineStr"/>
-      <c r="H91" t="inlineStr"/>
-      <c r="I91" t="inlineStr"/>
-      <c r="J91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3546,14 +3122,11 @@
         <v>1</v>
       </c>
       <c r="F92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G92" t="inlineStr"/>
-      <c r="H92" t="inlineStr"/>
+        <v>58</v>
+      </c>
       <c r="I92" t="n">
         <v>1</v>
       </c>
-      <c r="J92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3580,14 +3153,11 @@
         <v>1</v>
       </c>
       <c r="F93" t="n">
-        <v>0</v>
-      </c>
-      <c r="G93" t="inlineStr"/>
-      <c r="H93" t="inlineStr"/>
+        <v>250</v>
+      </c>
       <c r="I93" t="n">
         <v>1</v>
       </c>
-      <c r="J93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3611,17 +3181,11 @@
         </is>
       </c>
       <c r="E94" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" t="n">
-        <v>0</v>
-      </c>
-      <c r="G94" t="inlineStr"/>
-      <c r="H94" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I94" t="n">
         <v>1</v>
       </c>
-      <c r="J94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3645,17 +3209,11 @@
         </is>
       </c>
       <c r="E95" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" t="n">
-        <v>0</v>
-      </c>
-      <c r="G95" t="inlineStr"/>
-      <c r="H95" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I95" t="n">
         <v>1</v>
       </c>
-      <c r="J95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3681,11 +3239,6 @@
       <c r="E96" t="b">
         <v>0</v>
       </c>
-      <c r="F96" t="inlineStr"/>
-      <c r="G96" t="inlineStr"/>
-      <c r="H96" t="inlineStr"/>
-      <c r="I96" t="inlineStr"/>
-      <c r="J96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3714,8 +3267,6 @@
       <c r="F97" t="n">
         <v>4</v>
       </c>
-      <c r="G97" t="inlineStr"/>
-      <c r="H97" t="inlineStr"/>
       <c r="I97" t="n">
         <v>1</v>
       </c>
@@ -3752,8 +3303,6 @@
       <c r="F98" t="n">
         <v>15</v>
       </c>
-      <c r="G98" t="inlineStr"/>
-      <c r="H98" t="inlineStr"/>
       <c r="I98" t="n">
         <v>1</v>
       </c>
@@ -3785,17 +3334,11 @@
         </is>
       </c>
       <c r="E99" t="b">
-        <v>1</v>
-      </c>
-      <c r="F99" t="n">
-        <v>0</v>
-      </c>
-      <c r="G99" t="inlineStr"/>
-      <c r="H99" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I99" t="n">
         <v>1</v>
       </c>
-      <c r="J99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3819,17 +3362,11 @@
         </is>
       </c>
       <c r="E100" t="b">
-        <v>1</v>
-      </c>
-      <c r="F100" t="n">
-        <v>0</v>
-      </c>
-      <c r="G100" t="inlineStr"/>
-      <c r="H100" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I100" t="n">
         <v>1</v>
       </c>
-      <c r="J100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3855,11 +3392,6 @@
       <c r="E101" t="b">
         <v>0</v>
       </c>
-      <c r="F101" t="inlineStr"/>
-      <c r="G101" t="inlineStr"/>
-      <c r="H101" t="inlineStr"/>
-      <c r="I101" t="inlineStr"/>
-      <c r="J101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3888,8 +3420,6 @@
       <c r="F102" t="n">
         <v>29</v>
       </c>
-      <c r="G102" t="inlineStr"/>
-      <c r="H102" t="inlineStr"/>
       <c r="I102" t="n">
         <v>1</v>
       </c>
@@ -3926,8 +3456,6 @@
       <c r="F103" t="n">
         <v>250</v>
       </c>
-      <c r="G103" t="inlineStr"/>
-      <c r="H103" t="inlineStr"/>
       <c r="I103" t="n">
         <v>1</v>
       </c>
@@ -3959,17 +3487,11 @@
         </is>
       </c>
       <c r="E104" t="b">
-        <v>1</v>
-      </c>
-      <c r="F104" t="n">
-        <v>0</v>
-      </c>
-      <c r="G104" t="inlineStr"/>
-      <c r="H104" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I104" t="n">
         <v>1</v>
       </c>
-      <c r="J104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3993,17 +3515,11 @@
         </is>
       </c>
       <c r="E105" t="b">
-        <v>1</v>
-      </c>
-      <c r="F105" t="n">
-        <v>0</v>
-      </c>
-      <c r="G105" t="inlineStr"/>
-      <c r="H105" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I105" t="n">
         <v>1</v>
       </c>
-      <c r="J105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4029,11 +3545,6 @@
       <c r="E106" t="b">
         <v>0</v>
       </c>
-      <c r="F106" t="inlineStr"/>
-      <c r="G106" t="inlineStr"/>
-      <c r="H106" t="inlineStr"/>
-      <c r="I106" t="inlineStr"/>
-      <c r="J106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4060,14 +3571,11 @@
         <v>1</v>
       </c>
       <c r="F107" t="n">
-        <v>0</v>
-      </c>
-      <c r="G107" t="inlineStr"/>
-      <c r="H107" t="inlineStr"/>
+        <v>29</v>
+      </c>
       <c r="I107" t="n">
         <v>1</v>
       </c>
-      <c r="J107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4094,14 +3602,11 @@
         <v>1</v>
       </c>
       <c r="F108" t="n">
-        <v>0</v>
-      </c>
-      <c r="G108" t="inlineStr"/>
-      <c r="H108" t="inlineStr"/>
+        <v>250</v>
+      </c>
       <c r="I108" t="n">
         <v>1</v>
       </c>
-      <c r="J108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4125,17 +3630,11 @@
         </is>
       </c>
       <c r="E109" t="b">
-        <v>1</v>
-      </c>
-      <c r="F109" t="n">
-        <v>0</v>
-      </c>
-      <c r="G109" t="inlineStr"/>
-      <c r="H109" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I109" t="n">
         <v>1</v>
       </c>
-      <c r="J109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4159,17 +3658,11 @@
         </is>
       </c>
       <c r="E110" t="b">
-        <v>1</v>
-      </c>
-      <c r="F110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G110" t="inlineStr"/>
-      <c r="H110" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I110" t="n">
         <v>1</v>
       </c>
-      <c r="J110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4195,11 +3688,6 @@
       <c r="E111" t="b">
         <v>0</v>
       </c>
-      <c r="F111" t="inlineStr"/>
-      <c r="G111" t="inlineStr"/>
-      <c r="H111" t="inlineStr"/>
-      <c r="I111" t="inlineStr"/>
-      <c r="J111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4228,8 +3716,6 @@
       <c r="F112" t="n">
         <v>29</v>
       </c>
-      <c r="G112" t="inlineStr"/>
-      <c r="H112" t="inlineStr"/>
       <c r="I112" t="n">
         <v>1</v>
       </c>
@@ -4266,8 +3752,6 @@
       <c r="F113" t="n">
         <v>250</v>
       </c>
-      <c r="G113" t="inlineStr"/>
-      <c r="H113" t="inlineStr"/>
       <c r="I113" t="n">
         <v>1</v>
       </c>
@@ -4299,17 +3783,11 @@
         </is>
       </c>
       <c r="E114" t="b">
-        <v>1</v>
-      </c>
-      <c r="F114" t="n">
-        <v>0</v>
-      </c>
-      <c r="G114" t="inlineStr"/>
-      <c r="H114" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I114" t="n">
         <v>1</v>
       </c>
-      <c r="J114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4333,17 +3811,11 @@
         </is>
       </c>
       <c r="E115" t="b">
-        <v>1</v>
-      </c>
-      <c r="F115" t="n">
-        <v>0</v>
-      </c>
-      <c r="G115" t="inlineStr"/>
-      <c r="H115" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I115" t="n">
         <v>1</v>
       </c>
-      <c r="J115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4369,11 +3841,6 @@
       <c r="E116" t="b">
         <v>0</v>
       </c>
-      <c r="F116" t="inlineStr"/>
-      <c r="G116" t="inlineStr"/>
-      <c r="H116" t="inlineStr"/>
-      <c r="I116" t="inlineStr"/>
-      <c r="J116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4402,8 +3869,6 @@
       <c r="F117" t="n">
         <v>6</v>
       </c>
-      <c r="G117" t="inlineStr"/>
-      <c r="H117" t="inlineStr"/>
       <c r="I117" t="n">
         <v>1</v>
       </c>
@@ -4440,8 +3905,6 @@
       <c r="F118" t="n">
         <v>50</v>
       </c>
-      <c r="G118" t="inlineStr"/>
-      <c r="H118" t="inlineStr"/>
       <c r="I118" t="n">
         <v>1</v>
       </c>
@@ -4473,17 +3936,11 @@
         </is>
       </c>
       <c r="E119" t="b">
-        <v>1</v>
-      </c>
-      <c r="F119" t="n">
-        <v>0</v>
-      </c>
-      <c r="G119" t="inlineStr"/>
-      <c r="H119" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I119" t="n">
         <v>1</v>
       </c>
-      <c r="J119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -4507,17 +3964,11 @@
         </is>
       </c>
       <c r="E120" t="b">
-        <v>1</v>
-      </c>
-      <c r="F120" t="n">
-        <v>0</v>
-      </c>
-      <c r="G120" t="inlineStr"/>
-      <c r="H120" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I120" t="n">
         <v>1</v>
       </c>
-      <c r="J120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -4543,11 +3994,6 @@
       <c r="E121" t="b">
         <v>0</v>
       </c>
-      <c r="F121" t="inlineStr"/>
-      <c r="G121" t="inlineStr"/>
-      <c r="H121" t="inlineStr"/>
-      <c r="I121" t="inlineStr"/>
-      <c r="J121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -4576,8 +4022,6 @@
       <c r="F122" t="n">
         <v>2</v>
       </c>
-      <c r="G122" t="inlineStr"/>
-      <c r="H122" t="inlineStr"/>
       <c r="I122" t="n">
         <v>1</v>
       </c>
@@ -4614,8 +4058,6 @@
       <c r="F123" t="n">
         <v>10</v>
       </c>
-      <c r="G123" t="inlineStr"/>
-      <c r="H123" t="inlineStr"/>
       <c r="I123" t="n">
         <v>1</v>
       </c>
@@ -4647,17 +4089,11 @@
         </is>
       </c>
       <c r="E124" t="b">
-        <v>1</v>
-      </c>
-      <c r="F124" t="n">
-        <v>0</v>
-      </c>
-      <c r="G124" t="inlineStr"/>
-      <c r="H124" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I124" t="n">
         <v>1</v>
       </c>
-      <c r="J124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -4681,17 +4117,11 @@
         </is>
       </c>
       <c r="E125" t="b">
-        <v>1</v>
-      </c>
-      <c r="F125" t="n">
-        <v>0</v>
-      </c>
-      <c r="G125" t="inlineStr"/>
-      <c r="H125" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I125" t="n">
         <v>1</v>
       </c>
-      <c r="J125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -4717,11 +4147,6 @@
       <c r="E126" t="b">
         <v>0</v>
       </c>
-      <c r="F126" t="inlineStr"/>
-      <c r="G126" t="inlineStr"/>
-      <c r="H126" t="inlineStr"/>
-      <c r="I126" t="inlineStr"/>
-      <c r="J126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -4748,14 +4173,11 @@
         <v>1</v>
       </c>
       <c r="F127" t="n">
-        <v>0</v>
-      </c>
-      <c r="G127" t="inlineStr"/>
-      <c r="H127" t="inlineStr"/>
+        <v>345</v>
+      </c>
       <c r="I127" t="n">
         <v>1</v>
       </c>
-      <c r="J127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -4782,14 +4204,11 @@
         <v>1</v>
       </c>
       <c r="F128" t="n">
-        <v>0</v>
-      </c>
-      <c r="G128" t="inlineStr"/>
-      <c r="H128" t="inlineStr"/>
+        <v>3000</v>
+      </c>
       <c r="I128" t="n">
         <v>1</v>
       </c>
-      <c r="J128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -4813,17 +4232,11 @@
         </is>
       </c>
       <c r="E129" t="b">
-        <v>1</v>
-      </c>
-      <c r="F129" t="n">
-        <v>0</v>
-      </c>
-      <c r="G129" t="inlineStr"/>
-      <c r="H129" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I129" t="n">
         <v>1</v>
       </c>
-      <c r="J129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -4847,17 +4260,11 @@
         </is>
       </c>
       <c r="E130" t="b">
-        <v>1</v>
-      </c>
-      <c r="F130" t="n">
-        <v>0</v>
-      </c>
-      <c r="G130" t="inlineStr"/>
-      <c r="H130" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I130" t="n">
         <v>1</v>
       </c>
-      <c r="J130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -4883,11 +4290,6 @@
       <c r="E131" t="b">
         <v>0</v>
       </c>
-      <c r="F131" t="inlineStr"/>
-      <c r="G131" t="inlineStr"/>
-      <c r="H131" t="inlineStr"/>
-      <c r="I131" t="inlineStr"/>
-      <c r="J131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -4916,8 +4318,6 @@
       <c r="F132" t="n">
         <v>29</v>
       </c>
-      <c r="G132" t="inlineStr"/>
-      <c r="H132" t="inlineStr"/>
       <c r="I132" t="n">
         <v>1</v>
       </c>
@@ -4954,8 +4354,6 @@
       <c r="F133" t="n">
         <v>250</v>
       </c>
-      <c r="G133" t="inlineStr"/>
-      <c r="H133" t="inlineStr"/>
       <c r="I133" t="n">
         <v>1</v>
       </c>
@@ -4987,17 +4385,11 @@
         </is>
       </c>
       <c r="E134" t="b">
-        <v>1</v>
-      </c>
-      <c r="F134" t="n">
-        <v>0</v>
-      </c>
-      <c r="G134" t="inlineStr"/>
-      <c r="H134" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I134" t="n">
         <v>1</v>
       </c>
-      <c r="J134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5021,17 +4413,11 @@
         </is>
       </c>
       <c r="E135" t="b">
-        <v>1</v>
-      </c>
-      <c r="F135" t="n">
-        <v>0</v>
-      </c>
-      <c r="G135" t="inlineStr"/>
-      <c r="H135" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I135" t="n">
         <v>1</v>
       </c>
-      <c r="J135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -5057,11 +4443,6 @@
       <c r="E136" t="b">
         <v>0</v>
       </c>
-      <c r="F136" t="inlineStr"/>
-      <c r="G136" t="inlineStr"/>
-      <c r="H136" t="inlineStr"/>
-      <c r="I136" t="inlineStr"/>
-      <c r="J136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -5090,8 +4471,6 @@
       <c r="F137" t="n">
         <v>29</v>
       </c>
-      <c r="G137" t="inlineStr"/>
-      <c r="H137" t="inlineStr"/>
       <c r="I137" t="n">
         <v>1</v>
       </c>
@@ -5128,8 +4507,6 @@
       <c r="F138" t="n">
         <v>250</v>
       </c>
-      <c r="G138" t="inlineStr"/>
-      <c r="H138" t="inlineStr"/>
       <c r="I138" t="n">
         <v>1</v>
       </c>
@@ -5161,17 +4538,11 @@
         </is>
       </c>
       <c r="E139" t="b">
-        <v>1</v>
-      </c>
-      <c r="F139" t="n">
-        <v>0</v>
-      </c>
-      <c r="G139" t="inlineStr"/>
-      <c r="H139" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I139" t="n">
         <v>1</v>
       </c>
-      <c r="J139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5195,17 +4566,11 @@
         </is>
       </c>
       <c r="E140" t="b">
-        <v>1</v>
-      </c>
-      <c r="F140" t="n">
-        <v>0</v>
-      </c>
-      <c r="G140" t="inlineStr"/>
-      <c r="H140" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I140" t="n">
         <v>1</v>
       </c>
-      <c r="J140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5231,11 +4596,6 @@
       <c r="E141" t="b">
         <v>0</v>
       </c>
-      <c r="F141" t="inlineStr"/>
-      <c r="G141" t="inlineStr"/>
-      <c r="H141" t="inlineStr"/>
-      <c r="I141" t="inlineStr"/>
-      <c r="J141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -5262,14 +4622,11 @@
         <v>1</v>
       </c>
       <c r="F142" t="n">
-        <v>0</v>
-      </c>
-      <c r="G142" t="inlineStr"/>
-      <c r="H142" t="inlineStr"/>
+        <v>6</v>
+      </c>
       <c r="I142" t="n">
         <v>1</v>
       </c>
-      <c r="J142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -5296,14 +4653,11 @@
         <v>1</v>
       </c>
       <c r="F143" t="n">
-        <v>0</v>
-      </c>
-      <c r="G143" t="inlineStr"/>
-      <c r="H143" t="inlineStr"/>
+        <v>50</v>
+      </c>
       <c r="I143" t="n">
         <v>1</v>
       </c>
-      <c r="J143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -5327,17 +4681,11 @@
         </is>
       </c>
       <c r="E144" t="b">
-        <v>1</v>
-      </c>
-      <c r="F144" t="n">
-        <v>0</v>
-      </c>
-      <c r="G144" t="inlineStr"/>
-      <c r="H144" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I144" t="n">
         <v>1</v>
       </c>
-      <c r="J144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -5361,17 +4709,11 @@
         </is>
       </c>
       <c r="E145" t="b">
-        <v>1</v>
-      </c>
-      <c r="F145" t="n">
-        <v>0</v>
-      </c>
-      <c r="G145" t="inlineStr"/>
-      <c r="H145" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I145" t="n">
         <v>1</v>
       </c>
-      <c r="J145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -5397,11 +4739,6 @@
       <c r="E146" t="b">
         <v>0</v>
       </c>
-      <c r="F146" t="inlineStr"/>
-      <c r="G146" t="inlineStr"/>
-      <c r="H146" t="inlineStr"/>
-      <c r="I146" t="inlineStr"/>
-      <c r="J146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -5425,17 +4762,11 @@
         </is>
       </c>
       <c r="E147" t="b">
-        <v>1</v>
-      </c>
-      <c r="F147" t="n">
-        <v>0</v>
-      </c>
-      <c r="G147" t="inlineStr"/>
-      <c r="H147" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I147" t="n">
         <v>1</v>
       </c>
-      <c r="J147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -5459,17 +4790,11 @@
         </is>
       </c>
       <c r="E148" t="b">
-        <v>1</v>
-      </c>
-      <c r="F148" t="n">
-        <v>0</v>
-      </c>
-      <c r="G148" t="inlineStr"/>
-      <c r="H148" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I148" t="n">
         <v>1</v>
       </c>
-      <c r="J148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -5496,14 +4821,11 @@
         <v>1</v>
       </c>
       <c r="F149" t="n">
-        <v>0</v>
-      </c>
-      <c r="G149" t="inlineStr"/>
-      <c r="H149" t="inlineStr"/>
+        <v>1050</v>
+      </c>
       <c r="I149" t="n">
         <v>1</v>
       </c>
-      <c r="J149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -5527,17 +4849,11 @@
         </is>
       </c>
       <c r="E150" t="b">
-        <v>1</v>
-      </c>
-      <c r="F150" t="n">
-        <v>0</v>
-      </c>
-      <c r="G150" t="inlineStr"/>
-      <c r="H150" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I150" t="n">
         <v>1</v>
       </c>
-      <c r="J150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -5563,11 +4879,6 @@
       <c r="E151" t="b">
         <v>0</v>
       </c>
-      <c r="F151" t="inlineStr"/>
-      <c r="G151" t="inlineStr"/>
-      <c r="H151" t="inlineStr"/>
-      <c r="I151" t="inlineStr"/>
-      <c r="J151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -5591,17 +4902,11 @@
         </is>
       </c>
       <c r="E152" t="b">
-        <v>1</v>
-      </c>
-      <c r="F152" t="n">
-        <v>0</v>
-      </c>
-      <c r="G152" t="inlineStr"/>
-      <c r="H152" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I152" t="n">
         <v>1</v>
       </c>
-      <c r="J152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -5625,17 +4930,11 @@
         </is>
       </c>
       <c r="E153" t="b">
-        <v>1</v>
-      </c>
-      <c r="F153" t="n">
-        <v>0</v>
-      </c>
-      <c r="G153" t="inlineStr"/>
-      <c r="H153" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I153" t="n">
         <v>1</v>
       </c>
-      <c r="J153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -5662,14 +4961,11 @@
         <v>1</v>
       </c>
       <c r="F154" t="n">
-        <v>0</v>
-      </c>
-      <c r="G154" t="inlineStr"/>
-      <c r="H154" t="inlineStr"/>
+        <v>850</v>
+      </c>
       <c r="I154" t="n">
         <v>1</v>
       </c>
-      <c r="J154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -5693,17 +4989,11 @@
         </is>
       </c>
       <c r="E155" t="b">
-        <v>1</v>
-      </c>
-      <c r="F155" t="n">
-        <v>0</v>
-      </c>
-      <c r="G155" t="inlineStr"/>
-      <c r="H155" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I155" t="n">
         <v>1</v>
       </c>
-      <c r="J155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -5729,11 +5019,6 @@
       <c r="E156" t="b">
         <v>0</v>
       </c>
-      <c r="F156" t="inlineStr"/>
-      <c r="G156" t="inlineStr"/>
-      <c r="H156" t="inlineStr"/>
-      <c r="I156" t="inlineStr"/>
-      <c r="J156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -5762,8 +5047,6 @@
       <c r="F157" t="n">
         <v>5</v>
       </c>
-      <c r="G157" t="inlineStr"/>
-      <c r="H157" t="inlineStr"/>
       <c r="I157" t="n">
         <v>1</v>
       </c>
@@ -5800,8 +5083,6 @@
       <c r="F158" t="n">
         <v>13</v>
       </c>
-      <c r="G158" t="inlineStr"/>
-      <c r="H158" t="inlineStr"/>
       <c r="I158" t="n">
         <v>1</v>
       </c>
@@ -5833,17 +5114,11 @@
         </is>
       </c>
       <c r="E159" t="b">
-        <v>1</v>
-      </c>
-      <c r="F159" t="n">
-        <v>0</v>
-      </c>
-      <c r="G159" t="inlineStr"/>
-      <c r="H159" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I159" t="n">
         <v>1</v>
       </c>
-      <c r="J159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -5867,17 +5142,11 @@
         </is>
       </c>
       <c r="E160" t="b">
-        <v>1</v>
-      </c>
-      <c r="F160" t="n">
-        <v>0</v>
-      </c>
-      <c r="G160" t="inlineStr"/>
-      <c r="H160" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I160" t="n">
         <v>1</v>
       </c>
-      <c r="J160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -5903,11 +5172,6 @@
       <c r="E161" t="b">
         <v>0</v>
       </c>
-      <c r="F161" t="inlineStr"/>
-      <c r="G161" t="inlineStr"/>
-      <c r="H161" t="inlineStr"/>
-      <c r="I161" t="inlineStr"/>
-      <c r="J161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -5936,8 +5200,6 @@
       <c r="F162" t="n">
         <v>69</v>
       </c>
-      <c r="G162" t="inlineStr"/>
-      <c r="H162" t="inlineStr"/>
       <c r="I162" t="n">
         <v>1</v>
       </c>
@@ -5974,8 +5236,6 @@
       <c r="F163" t="n">
         <v>375</v>
       </c>
-      <c r="G163" t="inlineStr"/>
-      <c r="H163" t="inlineStr"/>
       <c r="I163" t="n">
         <v>1</v>
       </c>
@@ -6007,17 +5267,11 @@
         </is>
       </c>
       <c r="E164" t="b">
-        <v>1</v>
-      </c>
-      <c r="F164" t="n">
-        <v>0</v>
-      </c>
-      <c r="G164" t="inlineStr"/>
-      <c r="H164" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I164" t="n">
         <v>1</v>
       </c>
-      <c r="J164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -6041,17 +5295,11 @@
         </is>
       </c>
       <c r="E165" t="b">
-        <v>1</v>
-      </c>
-      <c r="F165" t="n">
-        <v>0</v>
-      </c>
-      <c r="G165" t="inlineStr"/>
-      <c r="H165" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I165" t="n">
         <v>1</v>
       </c>
-      <c r="J165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -6077,11 +5325,6 @@
       <c r="E166" t="b">
         <v>0</v>
       </c>
-      <c r="F166" t="inlineStr"/>
-      <c r="G166" t="inlineStr"/>
-      <c r="H166" t="inlineStr"/>
-      <c r="I166" t="inlineStr"/>
-      <c r="J166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -6108,14 +5351,11 @@
         <v>1</v>
       </c>
       <c r="F167" t="n">
-        <v>0</v>
-      </c>
-      <c r="G167" t="inlineStr"/>
-      <c r="H167" t="inlineStr"/>
+        <v>3</v>
+      </c>
       <c r="I167" t="n">
         <v>0</v>
       </c>
-      <c r="J167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -6142,14 +5382,11 @@
         <v>1</v>
       </c>
       <c r="F168" t="n">
-        <v>0</v>
-      </c>
-      <c r="G168" t="inlineStr"/>
-      <c r="H168" t="inlineStr"/>
+        <v>4</v>
+      </c>
       <c r="I168" t="n">
         <v>0</v>
       </c>
-      <c r="J168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -6173,17 +5410,11 @@
         </is>
       </c>
       <c r="E169" t="b">
-        <v>1</v>
-      </c>
-      <c r="F169" t="n">
-        <v>0</v>
-      </c>
-      <c r="G169" t="inlineStr"/>
-      <c r="H169" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I169" t="n">
         <v>1</v>
       </c>
-      <c r="J169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -6207,17 +5438,11 @@
         </is>
       </c>
       <c r="E170" t="b">
-        <v>1</v>
-      </c>
-      <c r="F170" t="n">
-        <v>0</v>
-      </c>
-      <c r="G170" t="inlineStr"/>
-      <c r="H170" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I170" t="n">
         <v>1</v>
       </c>
-      <c r="J170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -6243,11 +5468,6 @@
       <c r="E171" t="b">
         <v>0</v>
       </c>
-      <c r="F171" t="inlineStr"/>
-      <c r="G171" t="inlineStr"/>
-      <c r="H171" t="inlineStr"/>
-      <c r="I171" t="inlineStr"/>
-      <c r="J171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -6274,14 +5494,11 @@
         <v>1</v>
       </c>
       <c r="F172" t="n">
-        <v>0</v>
-      </c>
-      <c r="G172" t="inlineStr"/>
-      <c r="H172" t="inlineStr"/>
+        <v>1</v>
+      </c>
       <c r="I172" t="n">
         <v>1</v>
       </c>
-      <c r="J172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -6308,14 +5525,11 @@
         <v>1</v>
       </c>
       <c r="F173" t="n">
-        <v>0</v>
-      </c>
-      <c r="G173" t="inlineStr"/>
-      <c r="H173" t="inlineStr"/>
+        <v>1</v>
+      </c>
       <c r="I173" t="n">
         <v>1</v>
       </c>
-      <c r="J173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -6339,17 +5553,11 @@
         </is>
       </c>
       <c r="E174" t="b">
-        <v>1</v>
-      </c>
-      <c r="F174" t="n">
-        <v>0</v>
-      </c>
-      <c r="G174" t="inlineStr"/>
-      <c r="H174" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I174" t="n">
         <v>1</v>
       </c>
-      <c r="J174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -6373,17 +5581,11 @@
         </is>
       </c>
       <c r="E175" t="b">
-        <v>1</v>
-      </c>
-      <c r="F175" t="n">
-        <v>0</v>
-      </c>
-      <c r="G175" t="inlineStr"/>
-      <c r="H175" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I175" t="n">
         <v>1</v>
       </c>
-      <c r="J175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -6409,11 +5611,6 @@
       <c r="E176" t="b">
         <v>0</v>
       </c>
-      <c r="F176" t="inlineStr"/>
-      <c r="G176" t="inlineStr"/>
-      <c r="H176" t="inlineStr"/>
-      <c r="I176" t="inlineStr"/>
-      <c r="J176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -6437,17 +5634,11 @@
         </is>
       </c>
       <c r="E177" t="b">
-        <v>1</v>
-      </c>
-      <c r="F177" t="n">
-        <v>0</v>
-      </c>
-      <c r="G177" t="inlineStr"/>
-      <c r="H177" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I177" t="n">
         <v>1</v>
       </c>
-      <c r="J177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -6471,17 +5662,11 @@
         </is>
       </c>
       <c r="E178" t="b">
-        <v>1</v>
-      </c>
-      <c r="F178" t="n">
-        <v>0</v>
-      </c>
-      <c r="G178" t="inlineStr"/>
-      <c r="H178" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I178" t="n">
         <v>1</v>
       </c>
-      <c r="J178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -6505,17 +5690,11 @@
         </is>
       </c>
       <c r="E179" t="b">
-        <v>1</v>
-      </c>
-      <c r="F179" t="n">
-        <v>0</v>
-      </c>
-      <c r="G179" t="inlineStr"/>
-      <c r="H179" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I179" t="n">
         <v>1</v>
       </c>
-      <c r="J179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -6542,14 +5721,11 @@
         <v>1</v>
       </c>
       <c r="F180" t="n">
-        <v>0</v>
-      </c>
-      <c r="G180" t="inlineStr"/>
-      <c r="H180" t="inlineStr"/>
+        <v>1</v>
+      </c>
       <c r="I180" t="n">
         <v>1</v>
       </c>
-      <c r="J180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -6575,11 +5751,6 @@
       <c r="E181" t="b">
         <v>0</v>
       </c>
-      <c r="F181" t="inlineStr"/>
-      <c r="G181" t="inlineStr"/>
-      <c r="H181" t="inlineStr"/>
-      <c r="I181" t="inlineStr"/>
-      <c r="J181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -6603,17 +5774,11 @@
         </is>
       </c>
       <c r="E182" t="b">
-        <v>1</v>
-      </c>
-      <c r="F182" t="n">
-        <v>0</v>
-      </c>
-      <c r="G182" t="inlineStr"/>
-      <c r="H182" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I182" t="n">
         <v>1</v>
       </c>
-      <c r="J182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -6637,17 +5802,11 @@
         </is>
       </c>
       <c r="E183" t="b">
-        <v>1</v>
-      </c>
-      <c r="F183" t="n">
-        <v>0</v>
-      </c>
-      <c r="G183" t="inlineStr"/>
-      <c r="H183" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I183" t="n">
         <v>1</v>
       </c>
-      <c r="J183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -6671,17 +5830,11 @@
         </is>
       </c>
       <c r="E184" t="b">
-        <v>1</v>
-      </c>
-      <c r="F184" t="n">
-        <v>0</v>
-      </c>
-      <c r="G184" t="inlineStr"/>
-      <c r="H184" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I184" t="n">
         <v>1</v>
       </c>
-      <c r="J184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -6705,17 +5858,11 @@
         </is>
       </c>
       <c r="E185" t="b">
-        <v>1</v>
-      </c>
-      <c r="F185" t="n">
-        <v>0</v>
-      </c>
-      <c r="G185" t="inlineStr"/>
-      <c r="H185" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="I185" t="n">
         <v>1</v>
       </c>
-      <c r="J185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -6739,13 +5886,11 @@
         </is>
       </c>
       <c r="E186" t="b">
-        <v>0</v>
-      </c>
-      <c r="F186" t="inlineStr"/>
-      <c r="G186" t="inlineStr"/>
-      <c r="H186" t="inlineStr"/>
-      <c r="I186" t="inlineStr"/>
-      <c r="J186" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="F186" t="n">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>